<commit_message>
Fixes en rutas cobrador-pedidos y entregador-pedidos
</commit_message>
<xml_diff>
--- a/PRODUCTOS_reales.xlsx
+++ b/PRODUCTOS_reales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="d:\Sistema\Descargas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sistema\Documentos\GitHub\Xpatl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4FA871-9CE5-4A49-9205-0D1BEA2D53A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A7E8C0-C62D-457C-8CEC-5530BC17BA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22305" yWindow="4050" windowWidth="12330" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21795" yWindow="3000" windowWidth="16200" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="productos(6914)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="346">
   <si>
     <t>Clave</t>
   </si>
@@ -1055,6 +1055,9 @@
   </si>
   <si>
     <t>Precio_lista</t>
+  </si>
+  <si>
+    <t>Descuento</t>
   </si>
 </sst>
 </file>
@@ -1895,15 +1898,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D174"/>
+  <dimension ref="A1:E174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1916,8 +1919,11 @@
       <c r="D1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1930,8 +1936,11 @@
       <c r="D2">
         <v>209.9</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1944,8 +1953,11 @@
       <c r="D3">
         <v>349.9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1958,8 +1970,11 @@
       <c r="D4">
         <v>349.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1972,8 +1987,11 @@
       <c r="D5">
         <v>349.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1986,8 +2004,11 @@
       <c r="D6">
         <v>769.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2000,8 +2021,11 @@
       <c r="D7">
         <v>649.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -2014,8 +2038,11 @@
       <c r="D8">
         <v>389.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2028,8 +2055,11 @@
       <c r="D9">
         <v>449.9</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2042,8 +2072,11 @@
       <c r="D10">
         <v>769.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2056,8 +2089,11 @@
       <c r="D11">
         <v>769.9</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -2070,8 +2106,11 @@
       <c r="D12">
         <v>359.9</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -2084,8 +2123,11 @@
       <c r="D13">
         <v>219.9</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2098,8 +2140,11 @@
       <c r="D14">
         <v>689.9</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -2112,8 +2157,11 @@
       <c r="D15">
         <v>219.9</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -2126,8 +2174,11 @@
       <c r="D16">
         <v>319.89999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -2140,8 +2191,11 @@
       <c r="D17">
         <v>409.9</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -2154,8 +2208,11 @@
       <c r="D18">
         <v>579.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -2168,8 +2225,11 @@
       <c r="D19">
         <v>389.9</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -2182,8 +2242,11 @@
       <c r="D20">
         <v>469.9</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -2196,8 +2259,11 @@
       <c r="D21">
         <v>479.9</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -2210,8 +2276,11 @@
       <c r="D22">
         <v>339.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -2224,8 +2293,11 @@
       <c r="D23">
         <v>279.89999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -2238,8 +2310,11 @@
       <c r="D24">
         <v>389.9</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>49</v>
       </c>
@@ -2252,8 +2327,11 @@
       <c r="D25">
         <v>349.9</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -2266,8 +2344,11 @@
       <c r="D26">
         <v>449.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>53</v>
       </c>
@@ -2280,8 +2361,11 @@
       <c r="D27">
         <v>309.89999999999998</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>55</v>
       </c>
@@ -2294,8 +2378,11 @@
       <c r="D28">
         <v>349.9</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -2308,8 +2395,11 @@
       <c r="D29">
         <v>359.9</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -2322,8 +2412,11 @@
       <c r="D30">
         <v>219.9</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -2336,8 +2429,11 @@
       <c r="D31">
         <v>499.9</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -2350,8 +2446,11 @@
       <c r="D32">
         <v>469.9</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -2364,8 +2463,11 @@
       <c r="D33">
         <v>549.9</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -2378,8 +2480,11 @@
       <c r="D34">
         <v>659.9</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -2392,8 +2497,11 @@
       <c r="D35">
         <v>659.9</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -2406,8 +2514,11 @@
       <c r="D36">
         <v>659.9</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -2420,8 +2531,11 @@
       <c r="D37">
         <v>169.9</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -2434,8 +2548,11 @@
       <c r="D38">
         <v>359.9</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -2448,8 +2565,11 @@
       <c r="D39">
         <v>219.9</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -2462,8 +2582,11 @@
       <c r="D40">
         <v>659.9</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -2476,8 +2599,11 @@
       <c r="D41">
         <v>899.9</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -2490,8 +2616,11 @@
       <c r="D42">
         <v>769.9</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -2504,8 +2633,11 @@
       <c r="D43">
         <v>799.9</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -2518,8 +2650,11 @@
       <c r="D44">
         <v>689.9</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -2532,8 +2667,11 @@
       <c r="D45">
         <v>439.9</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -2546,8 +2684,11 @@
       <c r="D46">
         <v>549.9</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>92</v>
       </c>
@@ -2560,8 +2701,11 @@
       <c r="D47">
         <v>219.9</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>94</v>
       </c>
@@ -2574,8 +2718,11 @@
       <c r="D48">
         <v>319.89999999999998</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>96</v>
       </c>
@@ -2588,8 +2735,11 @@
       <c r="D49">
         <v>439.9</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>98</v>
       </c>
@@ -2602,8 +2752,11 @@
       <c r="D50">
         <v>339.9</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -2616,8 +2769,11 @@
       <c r="D51">
         <v>349.9</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>102</v>
       </c>
@@ -2630,8 +2786,11 @@
       <c r="D52">
         <v>439.9</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>104</v>
       </c>
@@ -2644,8 +2803,11 @@
       <c r="D53">
         <v>1099.9000000000001</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>106</v>
       </c>
@@ -2658,8 +2820,11 @@
       <c r="D54">
         <v>83.99</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>108</v>
       </c>
@@ -2672,8 +2837,11 @@
       <c r="D55">
         <v>1009.9</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>110</v>
       </c>
@@ -2686,8 +2854,11 @@
       <c r="D56">
         <v>369.9</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>112</v>
       </c>
@@ -2700,8 +2871,11 @@
       <c r="D57">
         <v>199.9</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>113</v>
       </c>
@@ -2714,8 +2888,11 @@
       <c r="D58">
         <v>619.9</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>115</v>
       </c>
@@ -2728,8 +2905,11 @@
       <c r="D59">
         <v>425.9</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>117</v>
       </c>
@@ -2742,8 +2922,11 @@
       <c r="D60">
         <v>539.9</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>119</v>
       </c>
@@ -2756,8 +2939,11 @@
       <c r="D61">
         <v>1099.9000000000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>121</v>
       </c>
@@ -2770,8 +2956,11 @@
       <c r="D62">
         <v>339.9</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>123</v>
       </c>
@@ -2784,8 +2973,11 @@
       <c r="D63">
         <v>289.89999999999998</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>125</v>
       </c>
@@ -2798,8 +2990,11 @@
       <c r="D64">
         <v>379.9</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>127</v>
       </c>
@@ -2812,8 +3007,11 @@
       <c r="D65">
         <v>529.9</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>129</v>
       </c>
@@ -2826,8 +3024,11 @@
       <c r="D66">
         <v>469.9</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>131</v>
       </c>
@@ -2840,8 +3041,11 @@
       <c r="D67">
         <v>829.9</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>133</v>
       </c>
@@ -2854,8 +3058,11 @@
       <c r="D68">
         <v>369.9</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>135</v>
       </c>
@@ -2868,8 +3075,11 @@
       <c r="D69">
         <v>509.9</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>137</v>
       </c>
@@ -2882,8 +3092,11 @@
       <c r="D70">
         <v>409.9</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>139</v>
       </c>
@@ -2896,8 +3109,11 @@
       <c r="D71">
         <v>419.9</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>141</v>
       </c>
@@ -2910,8 +3126,11 @@
       <c r="D72">
         <v>269.89999999999998</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -2924,8 +3143,11 @@
       <c r="D73">
         <v>329.9</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -2938,8 +3160,11 @@
       <c r="D74">
         <v>659.9</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>145</v>
       </c>
@@ -2952,8 +3177,11 @@
       <c r="D75">
         <v>369.9</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>147</v>
       </c>
@@ -2966,8 +3194,11 @@
       <c r="D76">
         <v>489.9</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>149</v>
       </c>
@@ -2980,8 +3211,11 @@
       <c r="D77">
         <v>769.9</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>151</v>
       </c>
@@ -2994,8 +3228,11 @@
       <c r="D78">
         <v>619.9</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>153</v>
       </c>
@@ -3008,8 +3245,11 @@
       <c r="D79">
         <v>339.9</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>155</v>
       </c>
@@ -3022,8 +3262,11 @@
       <c r="D80">
         <v>309.89999999999998</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>157</v>
       </c>
@@ -3036,8 +3279,11 @@
       <c r="D81">
         <v>609.9</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>159</v>
       </c>
@@ -3050,8 +3296,11 @@
       <c r="D82">
         <v>429.9</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>161</v>
       </c>
@@ -3064,8 +3313,11 @@
       <c r="D83">
         <v>1249.9000000000001</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>163</v>
       </c>
@@ -3078,8 +3330,11 @@
       <c r="D84">
         <v>1399.9</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>165</v>
       </c>
@@ -3092,8 +3347,11 @@
       <c r="D85">
         <v>839.9</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>167</v>
       </c>
@@ -3106,8 +3364,11 @@
       <c r="D86">
         <v>439.9</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>169</v>
       </c>
@@ -3120,8 +3381,11 @@
       <c r="D87">
         <v>389.9</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>171</v>
       </c>
@@ -3134,8 +3398,11 @@
       <c r="D88">
         <v>549.9</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>173</v>
       </c>
@@ -3148,8 +3415,11 @@
       <c r="D89">
         <v>439.9</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>175</v>
       </c>
@@ -3162,8 +3432,11 @@
       <c r="D90">
         <v>319.89999999999998</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>177</v>
       </c>
@@ -3176,8 +3449,11 @@
       <c r="D91">
         <v>449.9</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>179</v>
       </c>
@@ -3190,8 +3466,11 @@
       <c r="D92">
         <v>959.9</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>181</v>
       </c>
@@ -3204,8 +3483,11 @@
       <c r="D93">
         <v>219.9</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>183</v>
       </c>
@@ -3218,8 +3500,11 @@
       <c r="D94">
         <v>319.89999999999998</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>184</v>
       </c>
@@ -3232,8 +3517,11 @@
       <c r="D95">
         <v>319.89999999999998</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>186</v>
       </c>
@@ -3246,8 +3534,11 @@
       <c r="D96">
         <v>609.9</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>188</v>
       </c>
@@ -3260,8 +3551,11 @@
       <c r="D97">
         <v>299.89999999999998</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>190</v>
       </c>
@@ -3274,8 +3568,11 @@
       <c r="D98">
         <v>359.9</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>192</v>
       </c>
@@ -3288,8 +3585,11 @@
       <c r="D99">
         <v>219.9</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>194</v>
       </c>
@@ -3302,8 +3602,11 @@
       <c r="D100">
         <v>399.9</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>196</v>
       </c>
@@ -3316,8 +3619,11 @@
       <c r="D101">
         <v>269.89999999999998</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>198</v>
       </c>
@@ -3330,8 +3636,11 @@
       <c r="D102">
         <v>329.9</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>200</v>
       </c>
@@ -3344,8 +3653,11 @@
       <c r="D103">
         <v>769.9</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>202</v>
       </c>
@@ -3358,8 +3670,11 @@
       <c r="D104">
         <v>499.9</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>204</v>
       </c>
@@ -3372,8 +3687,11 @@
       <c r="D105">
         <v>329.9</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E105">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>206</v>
       </c>
@@ -3386,8 +3704,11 @@
       <c r="D106">
         <v>449.9</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E106">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>208</v>
       </c>
@@ -3400,8 +3721,11 @@
       <c r="D107">
         <v>539.9</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E107">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>210</v>
       </c>
@@ -3414,8 +3738,11 @@
       <c r="D108">
         <v>249.99</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E108">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>212</v>
       </c>
@@ -3428,8 +3755,11 @@
       <c r="D109">
         <v>469.9</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E109">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>214</v>
       </c>
@@ -3442,8 +3772,11 @@
       <c r="D110">
         <v>899.9</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E110">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>216</v>
       </c>
@@ -3456,8 +3789,11 @@
       <c r="D111">
         <v>359.9</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E111">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>218</v>
       </c>
@@ -3470,8 +3806,11 @@
       <c r="D112">
         <v>469.9</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E112">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>220</v>
       </c>
@@ -3484,8 +3823,11 @@
       <c r="D113">
         <v>399.9</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E113">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>222</v>
       </c>
@@ -3498,8 +3840,11 @@
       <c r="D114">
         <v>399.9</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E114">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>224</v>
       </c>
@@ -3512,8 +3857,11 @@
       <c r="D115">
         <v>249.9</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E115">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>226</v>
       </c>
@@ -3526,8 +3874,11 @@
       <c r="D116">
         <v>359.9</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E116">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>228</v>
       </c>
@@ -3540,8 +3891,11 @@
       <c r="D117">
         <v>219.9</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E117">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>230</v>
       </c>
@@ -3554,8 +3908,11 @@
       <c r="D118">
         <v>359.9</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E118">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>232</v>
       </c>
@@ -3568,8 +3925,11 @@
       <c r="D119">
         <v>219.9</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E119">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>234</v>
       </c>
@@ -3582,8 +3942,11 @@
       <c r="D120">
         <v>419.9</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E120">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>236</v>
       </c>
@@ -3596,8 +3959,11 @@
       <c r="D121">
         <v>494.9</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E121">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>238</v>
       </c>
@@ -3610,8 +3976,11 @@
       <c r="D122">
         <v>439.9</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E122">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>240</v>
       </c>
@@ -3624,8 +3993,11 @@
       <c r="D123">
         <v>549.9</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E123">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>242</v>
       </c>
@@ -3638,8 +4010,11 @@
       <c r="D124">
         <v>309.89999999999998</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E124">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>244</v>
       </c>
@@ -3652,8 +4027,11 @@
       <c r="D125">
         <v>449.9</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E125">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>246</v>
       </c>
@@ -3666,8 +4044,11 @@
       <c r="D126">
         <v>689.9</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E126">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>248</v>
       </c>
@@ -3680,8 +4061,11 @@
       <c r="D127">
         <v>449.9</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E127">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>250</v>
       </c>
@@ -3694,8 +4078,11 @@
       <c r="D128">
         <v>379.9</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>252</v>
       </c>
@@ -3708,8 +4095,11 @@
       <c r="D129">
         <v>519.9</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>254</v>
       </c>
@@ -3722,8 +4112,11 @@
       <c r="D130">
         <v>349.9</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>256</v>
       </c>
@@ -3736,8 +4129,11 @@
       <c r="D131">
         <v>299.89999999999998</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>258</v>
       </c>
@@ -3750,8 +4146,11 @@
       <c r="D132">
         <v>499.9</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>260</v>
       </c>
@@ -3764,8 +4163,11 @@
       <c r="D133">
         <v>389.9</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>262</v>
       </c>
@@ -3778,8 +4180,11 @@
       <c r="D134">
         <v>299.89999999999998</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>264</v>
       </c>
@@ -3792,8 +4197,11 @@
       <c r="D135">
         <v>229.9</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E135">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>266</v>
       </c>
@@ -3806,8 +4214,11 @@
       <c r="D136">
         <v>279.89999999999998</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>268</v>
       </c>
@@ -3820,8 +4231,11 @@
       <c r="D137">
         <v>669.9</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E137">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>270</v>
       </c>
@@ -3834,8 +4248,11 @@
       <c r="D138">
         <v>359.9</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E138">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>272</v>
       </c>
@@ -3848,8 +4265,11 @@
       <c r="D139">
         <v>379.9</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E139">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>274</v>
       </c>
@@ -3862,8 +4282,11 @@
       <c r="D140">
         <v>659.9</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E140">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>276</v>
       </c>
@@ -3876,8 +4299,11 @@
       <c r="D141">
         <v>419.9</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>278</v>
       </c>
@@ -3890,8 +4316,11 @@
       <c r="D142">
         <v>409.9</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>280</v>
       </c>
@@ -3904,8 +4333,11 @@
       <c r="D143">
         <v>389.9</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E143">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>282</v>
       </c>
@@ -3918,8 +4350,11 @@
       <c r="D144">
         <v>419.9</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E144">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>284</v>
       </c>
@@ -3932,8 +4367,11 @@
       <c r="D145">
         <v>659.9</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E145">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>286</v>
       </c>
@@ -3946,8 +4384,11 @@
       <c r="D146">
         <v>659.9</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E146">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>288</v>
       </c>
@@ -3960,8 +4401,11 @@
       <c r="D147">
         <v>519.9</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E147">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>290</v>
       </c>
@@ -3974,8 +4418,11 @@
       <c r="D148">
         <v>429.9</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E148">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>292</v>
       </c>
@@ -3988,8 +4435,11 @@
       <c r="D149">
         <v>279.89999999999998</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E149">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>294</v>
       </c>
@@ -4002,8 +4452,11 @@
       <c r="D150">
         <v>499.9</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E150">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>296</v>
       </c>
@@ -4016,8 +4469,11 @@
       <c r="D151">
         <v>299.89999999999998</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E151">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>298</v>
       </c>
@@ -4030,8 +4486,11 @@
       <c r="D152">
         <v>429.9</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E152">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>300</v>
       </c>
@@ -4044,8 +4503,11 @@
       <c r="D153">
         <v>699.99</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E153">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>302</v>
       </c>
@@ -4058,8 +4520,11 @@
       <c r="D154">
         <v>279.89999999999998</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E154">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>304</v>
       </c>
@@ -4072,8 +4537,11 @@
       <c r="D155">
         <v>549.9</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E155">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>306</v>
       </c>
@@ -4086,8 +4554,11 @@
       <c r="D156">
         <v>419.9</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E156">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>308</v>
       </c>
@@ -4100,8 +4571,11 @@
       <c r="D157">
         <v>279.89999999999998</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E157">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>310</v>
       </c>
@@ -4114,8 +4588,11 @@
       <c r="D158">
         <v>329.9</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E158">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>312</v>
       </c>
@@ -4128,8 +4605,11 @@
       <c r="D159">
         <v>449.9</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E159">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>314</v>
       </c>
@@ -4142,8 +4622,11 @@
       <c r="D160">
         <v>519.9</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E160">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>316</v>
       </c>
@@ -4156,8 +4639,11 @@
       <c r="D161">
         <v>369.9</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E161">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>318</v>
       </c>
@@ -4170,8 +4656,11 @@
       <c r="D162">
         <v>769.9</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E162">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>320</v>
       </c>
@@ -4184,8 +4673,11 @@
       <c r="D163">
         <v>269.89999999999998</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E163">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>322</v>
       </c>
@@ -4198,8 +4690,11 @@
       <c r="D164">
         <v>199.9</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E164">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>324</v>
       </c>
@@ -4212,8 +4707,11 @@
       <c r="D165">
         <v>249.9</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E165">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>326</v>
       </c>
@@ -4226,8 +4724,11 @@
       <c r="D166">
         <v>279.89999999999998</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E166">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>328</v>
       </c>
@@ -4240,8 +4741,11 @@
       <c r="D167">
         <v>709.9</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E167">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>330</v>
       </c>
@@ -4254,8 +4758,11 @@
       <c r="D168">
         <v>339.9</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E168">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>332</v>
       </c>
@@ -4268,8 +4775,11 @@
       <c r="D169">
         <v>149.9</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E169">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>334</v>
       </c>
@@ -4282,8 +4792,11 @@
       <c r="D170">
         <v>839.9</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E170">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>336</v>
       </c>
@@ -4296,8 +4809,11 @@
       <c r="D171">
         <v>249.9</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E171">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>338</v>
       </c>
@@ -4310,8 +4826,11 @@
       <c r="D172">
         <v>1079.9000000000001</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E172">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>340</v>
       </c>
@@ -4324,8 +4843,11 @@
       <c r="D173">
         <v>1540</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E173">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>342</v>
       </c>
@@ -4337,6 +4859,9 @@
       </c>
       <c r="D174">
         <v>2520</v>
+      </c>
+      <c r="E174">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>